<commit_message>
Ops method work and other changes
</commit_message>
<xml_diff>
--- a/z_documents/Error Codes.xlsx
+++ b/z_documents/Error Codes.xlsx
@@ -12,23 +12,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>NUMBER CODE</t>
   </si>
   <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>NO ERROR</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>COMM ERROR</t>
+  </si>
+  <si>
+    <t>090</t>
+  </si>
+  <si>
+    <t>ERROR IN CODE CAUSED ERROR</t>
+  </si>
+  <si>
     <t>GENERAL CODES</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>DESC</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
     <t>TYPE/DESC</t>
   </si>
   <si>
@@ -41,99 +56,96 @@
     <t>0XX</t>
   </si>
   <si>
-    <t>NO ERROR</t>
-  </si>
-  <si>
     <t>SYSTEM ERROR</t>
   </si>
   <si>
-    <t>050</t>
-  </si>
-  <si>
     <t>BLINK FAST</t>
   </si>
   <si>
-    <t>COMM ERROR</t>
-  </si>
-  <si>
     <t>comm loss, keyboard loss, etc</t>
   </si>
   <si>
-    <t>090</t>
-  </si>
-  <si>
-    <t>ERROR IN CODE CAUSED ERROR</t>
+    <t>09X</t>
+  </si>
+  <si>
+    <t>CRITICAL SYSTEM ERROR</t>
+  </si>
+  <si>
+    <t>SOLID</t>
+  </si>
+  <si>
+    <t>1XX</t>
+  </si>
+  <si>
+    <t>GENERAL STOP ERRORS</t>
+  </si>
+  <si>
+    <t>BLINK 500</t>
+  </si>
+  <si>
+    <t>2XX</t>
+  </si>
+  <si>
+    <t>OPERATOR ERROR CAUSED ERRORS</t>
   </si>
   <si>
     <t>Check DEBUG messages for more info</t>
   </si>
   <si>
-    <t>09X</t>
-  </si>
-  <si>
-    <t>CRITICAL SYSTEM ERROR</t>
-  </si>
-  <si>
-    <t>SOLID</t>
-  </si>
-  <si>
-    <t>1XX</t>
-  </si>
-  <si>
-    <t>GENERAL STOP ERRORS</t>
+    <t>BLINK NORMAL</t>
+  </si>
+  <si>
+    <t>airgates, restraints toggled, etc.</t>
+  </si>
+  <si>
+    <t>3XX</t>
+  </si>
+  <si>
+    <t>MISC ERRORS</t>
+  </si>
+  <si>
+    <t>trevor error</t>
+  </si>
+  <si>
+    <t>4XX</t>
+  </si>
+  <si>
+    <t>STARTUP ERROR</t>
+  </si>
+  <si>
+    <t>5XX</t>
+  </si>
+  <si>
+    <t>RANDOM GENERATED ERRORS</t>
   </si>
   <si>
     <t>100</t>
   </si>
   <si>
-    <t>BLINK 500</t>
-  </si>
-  <si>
     <t>PANEL KEYED OFF</t>
   </si>
   <si>
     <t>PANEL POWER KEYSWITCH TURNED OFF</t>
   </si>
   <si>
-    <t>2XX</t>
-  </si>
-  <si>
     <t>101</t>
   </si>
   <si>
-    <t>OPERATOR ERROR CAUSED ERRORS</t>
-  </si>
-  <si>
-    <t>BLINK NORMAL</t>
-  </si>
-  <si>
     <t>PANEL KEYED OFF DURING OPS</t>
   </si>
   <si>
-    <t>airgates, restraints toggled, etc.</t>
-  </si>
-  <si>
     <t>PANEL POWER TURNED OFF WHILE ESR RESET</t>
   </si>
   <si>
-    <t>3XX</t>
-  </si>
-  <si>
     <t>110</t>
   </si>
   <si>
-    <t>MISC ERRORS</t>
-  </si>
-  <si>
     <t>RIDE TIMEOUT</t>
   </si>
   <si>
     <t>PANEL LEFT UNATTENDED FOR __ SECONDS</t>
   </si>
   <si>
-    <t>trevor error</t>
-  </si>
-  <si>
     <t>150</t>
   </si>
   <si>
@@ -219,6 +231,12 @@
   </si>
   <si>
     <t>Acknowledge button was pressed too many times while in auto mode</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>GENERAL STARTUP ERROR</t>
   </si>
 </sst>
 </file>
@@ -317,37 +335,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -364,51 +382,51 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14">
@@ -428,88 +446,88 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27">
@@ -523,20 +541,25 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="4"/>
+      <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4"/>
@@ -577,80 +600,96 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>